<commit_message>
Add extra info to distribution
</commit_message>
<xml_diff>
--- a/distribution.xlsx
+++ b/distribution.xlsx
@@ -676,7 +676,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:S126"/>
+  <dimension ref="A1:S132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A2" sqref="A2"/>
@@ -2928,6 +2928,225 @@
       </c>
       <c r="S126" t="str">
         <f>SUM(S1:S125)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19">
+      <c r="B130" t="s">
+        <v>20</v>
+      </c>
+      <c r="C130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",C2:C125)</f>
+        <v>0</v>
+      </c>
+      <c r="D130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",D2:D125)</f>
+        <v>0</v>
+      </c>
+      <c r="E130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",E2:E125)</f>
+        <v>0</v>
+      </c>
+      <c r="F130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",F2:F125)</f>
+        <v>0</v>
+      </c>
+      <c r="G130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",G2:G125)</f>
+        <v>0</v>
+      </c>
+      <c r="H130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",H2:H125)</f>
+        <v>0</v>
+      </c>
+      <c r="I130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",I2:I125)</f>
+        <v>0</v>
+      </c>
+      <c r="J130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",J2:J125)</f>
+        <v>0</v>
+      </c>
+      <c r="K130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",K2:K125)</f>
+        <v>0</v>
+      </c>
+      <c r="L130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",L2:L125)</f>
+        <v>0</v>
+      </c>
+      <c r="M130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",M2:M125)</f>
+        <v>0</v>
+      </c>
+      <c r="N130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",N2:N125)</f>
+        <v>0</v>
+      </c>
+      <c r="O130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",O2:O125)</f>
+        <v>0</v>
+      </c>
+      <c r="P130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",P2:P125)</f>
+        <v>0</v>
+      </c>
+      <c r="Q130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",Q2:Q125)</f>
+        <v>0</v>
+      </c>
+      <c r="R130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",R2:R125)</f>
+        <v>0</v>
+      </c>
+      <c r="S130" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектирование информационных систем;",S2:S125)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19">
+      <c r="B131" t="s">
+        <v>22</v>
+      </c>
+      <c r="C131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",C2:C125)</f>
+        <v>0</v>
+      </c>
+      <c r="D131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",D2:D125)</f>
+        <v>0</v>
+      </c>
+      <c r="E131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",E2:E125)</f>
+        <v>0</v>
+      </c>
+      <c r="F131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",F2:F125)</f>
+        <v>0</v>
+      </c>
+      <c r="G131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",G2:G125)</f>
+        <v>0</v>
+      </c>
+      <c r="H131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",H2:H125)</f>
+        <v>0</v>
+      </c>
+      <c r="I131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",I2:I125)</f>
+        <v>0</v>
+      </c>
+      <c r="J131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",J2:J125)</f>
+        <v>0</v>
+      </c>
+      <c r="K131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",K2:K125)</f>
+        <v>0</v>
+      </c>
+      <c r="L131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",L2:L125)</f>
+        <v>0</v>
+      </c>
+      <c r="M131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",M2:M125)</f>
+        <v>0</v>
+      </c>
+      <c r="N131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",N2:N125)</f>
+        <v>0</v>
+      </c>
+      <c r="O131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",O2:O125)</f>
+        <v>0</v>
+      </c>
+      <c r="P131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",P2:P125)</f>
+        <v>0</v>
+      </c>
+      <c r="Q131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",Q2:Q125)</f>
+        <v>0</v>
+      </c>
+      <c r="R131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",R2:R125)</f>
+        <v>0</v>
+      </c>
+      <c r="S131" t="str">
+        <f>SUMIF(B2:B125,"ПИ_Б;Проектный практикум;",S2:S125)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19">
+      <c r="B132" t="s">
+        <v>38</v>
+      </c>
+      <c r="C132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",C2:C125)</f>
+        <v>0</v>
+      </c>
+      <c r="D132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",D2:D125)</f>
+        <v>0</v>
+      </c>
+      <c r="E132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",E2:E125)</f>
+        <v>0</v>
+      </c>
+      <c r="F132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",F2:F125)</f>
+        <v>0</v>
+      </c>
+      <c r="G132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",G2:G125)</f>
+        <v>0</v>
+      </c>
+      <c r="H132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",H2:H125)</f>
+        <v>0</v>
+      </c>
+      <c r="I132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",I2:I125)</f>
+        <v>0</v>
+      </c>
+      <c r="J132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",J2:J125)</f>
+        <v>0</v>
+      </c>
+      <c r="K132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",K2:K125)</f>
+        <v>0</v>
+      </c>
+      <c r="L132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",L2:L125)</f>
+        <v>0</v>
+      </c>
+      <c r="M132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",M2:M125)</f>
+        <v>0</v>
+      </c>
+      <c r="N132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",N2:N125)</f>
+        <v>0</v>
+      </c>
+      <c r="O132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",O2:O125)</f>
+        <v>0</v>
+      </c>
+      <c r="P132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",P2:P125)</f>
+        <v>0</v>
+      </c>
+      <c r="Q132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",Q2:Q125)</f>
+        <v>0</v>
+      </c>
+      <c r="R132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",R2:R125)</f>
+        <v>0</v>
+      </c>
+      <c r="S132" t="str">
+        <f>SUMIF(B2:B125,"ПИ_М;Интеграция систем;",S2:S125)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>